<commit_message>
Raw data of CDRS flowers
</commit_message>
<xml_diff>
--- a/Data/Raw/Herbarium measurements flowers w leaf column_2021.xlsx
+++ b/Data/Raw/Herbarium measurements flowers w leaf column_2021.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23901"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Tiffani\Desktop\GRAD school\EvoEco Lab\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Daniel\Documents\R\Tribulus\Tribulus mericarp morphology\Tribulus-mericarp-morphology\Data\Raw\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4821CDD-46FF-433D-9E43-6BDFE6608DCB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67C1D688-BA02-4ED7-886E-955340297DD8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{947E4361-A4BF-6543-8AF9-EC67A39F65AD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{947E4361-A4BF-6543-8AF9-EC67A39F65AD}"/>
   </bookViews>
   <sheets>
     <sheet name="Flower" sheetId="1" r:id="rId1"/>
@@ -700,19 +700,19 @@
   <dimension ref="A1:L42"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O37" sqref="O37"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C38" sqref="C38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" style="7"/>
-    <col min="2" max="8" width="0" style="2" hidden="1" customWidth="1"/>
-    <col min="9" max="10" width="11.19921875" style="5"/>
-    <col min="11" max="16384" width="11.19921875" style="2"/>
+    <col min="1" max="1" width="11.25" style="7"/>
+    <col min="2" max="8" width="11.25" style="2" customWidth="1"/>
+    <col min="9" max="10" width="11.25" style="5"/>
+    <col min="11" max="16384" width="11.25" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
@@ -750,7 +750,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>92</v>
       </c>
@@ -767,7 +767,7 @@
         <v>4.3250999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1239</v>
       </c>
@@ -781,7 +781,7 @@
         <v>4.3253000000000004</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" s="7">
         <v>1239</v>
       </c>
@@ -795,7 +795,7 @@
         <v>4.3253000000000004</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -812,7 +812,7 @@
         <v>4.3135000000000003</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
         <v>23</v>
       </c>
@@ -829,7 +829,7 @@
         <v>4.3135000000000003</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>3184</v>
       </c>
@@ -843,7 +843,7 @@
         <v>4.3502000000000001</v>
       </c>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>3184</v>
       </c>
@@ -857,7 +857,7 @@
         <v>4.3502000000000001</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9" s="14">
         <v>3184</v>
       </c>
@@ -871,7 +871,7 @@
         <v>4.3502000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>4408</v>
       </c>
@@ -885,7 +885,7 @@
         <v>4.3159000000000001</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>6145</v>
       </c>
@@ -899,7 +899,7 @@
         <v>4.3143000000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12" s="9">
         <v>7475</v>
       </c>
@@ -913,7 +913,7 @@
         <v>4.3150000000000004</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13" s="9">
         <v>7599</v>
       </c>
@@ -930,7 +930,7 @@
         <v>17.288399999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14" s="9">
         <v>7611</v>
       </c>
@@ -947,7 +947,7 @@
         <v>17.303699999999999</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>7634</v>
       </c>
@@ -964,7 +964,7 @@
         <v>17.290700000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
         <v>28</v>
       </c>
@@ -978,7 +978,7 @@
         <v>17.2803</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
         <v>29</v>
       </c>
@@ -995,7 +995,7 @@
         <v>17.281300000000002</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
         <v>30</v>
       </c>
@@ -1012,7 +1012,7 @@
         <v>17.273700000000002</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
         <v>31</v>
       </c>
@@ -1029,7 +1029,7 @@
         <v>17.247599999999998</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
         <v>32</v>
       </c>
@@ -1046,7 +1046,7 @@
         <v>17.287299999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21" s="7">
         <v>9850</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>17.284199999999998</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22" s="7">
         <v>9961</v>
       </c>
@@ -1080,7 +1080,7 @@
         <v>17.264199999999999</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>9961</v>
       </c>
@@ -1097,7 +1097,7 @@
         <v>17.264199999999999</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24" s="7">
         <v>9974</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>17.292100000000001</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25" s="7">
         <v>9974</v>
       </c>
@@ -1125,7 +1125,7 @@
         <v>17.292100000000001</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26" s="7">
         <v>9974</v>
       </c>
@@ -1139,7 +1139,7 @@
         <v>17.292100000000001</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
         <v>35</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>17.3017</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
         <v>36</v>
       </c>
@@ -1173,7 +1173,7 @@
         <v>17.2883</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29" s="7">
         <v>13743</v>
       </c>
@@ -1190,7 +1190,7 @@
         <v>17.3033</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30" s="7">
         <v>16045</v>
       </c>
@@ -1207,7 +1207,7 @@
         <v>17.273399999999999</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31" s="7">
         <v>16356</v>
       </c>
@@ -1221,7 +1221,7 @@
         <v>17.295200000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32" s="7">
         <v>16356</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>17.295200000000001</v>
       </c>
     </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33" s="7">
         <v>16359</v>
       </c>
@@ -1252,7 +1252,7 @@
         <v>17.276900000000001</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
         <v>38</v>
       </c>
@@ -1266,7 +1266,7 @@
         <v>17.2668</v>
       </c>
     </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
         <v>38</v>
       </c>
@@ -1283,7 +1283,7 @@
         <v>17.2668</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36" s="7">
         <v>52794</v>
       </c>
@@ -1300,7 +1300,7 @@
         <v>17.279699999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37" s="7">
         <v>56362</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>17.2971</v>
       </c>
     </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42" s="17"/>
     </row>
   </sheetData>
@@ -1333,16 +1333,16 @@
       <selection activeCell="M16" sqref="M16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="11.19921875" style="9"/>
+    <col min="1" max="1" width="11.25" style="9"/>
     <col min="2" max="8" width="0" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="14.69921875" style="10" customWidth="1"/>
-    <col min="11" max="11" width="13.296875" customWidth="1"/>
-    <col min="17" max="17" width="10.796875" style="2"/>
+    <col min="10" max="10" width="14.75" style="10" customWidth="1"/>
+    <col min="11" max="11" width="13.25" customWidth="1"/>
+    <col min="17" max="17" width="10.75" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>7</v>
       </c>
@@ -1387,7 +1387,7 @@
       </c>
       <c r="O1" s="2"/>
     </row>
-    <row r="2" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A2" s="7">
         <v>1239</v>
       </c>
@@ -1459,7 +1459,7 @@
       <c r="BD2" s="2"/>
       <c r="BE2" s="2"/>
     </row>
-    <row r="3" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="7">
         <v>1239</v>
       </c>
@@ -1532,7 +1532,7 @@
       <c r="BD3" s="2"/>
       <c r="BE3" s="2"/>
     </row>
-    <row r="4" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
         <v>23</v>
       </c>
@@ -1605,7 +1605,7 @@
       <c r="BD4" s="2"/>
       <c r="BE4" s="2"/>
     </row>
-    <row r="5" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
         <v>23</v>
       </c>
@@ -1678,7 +1678,7 @@
       <c r="BD5" s="2"/>
       <c r="BE5" s="2"/>
     </row>
-    <row r="6" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="14">
         <v>3184</v>
       </c>
@@ -1701,7 +1701,7 @@
         <v>4.3502000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="14">
         <v>3184</v>
       </c>
@@ -1774,7 +1774,7 @@
       <c r="BD7" s="2"/>
       <c r="BE7" s="2"/>
     </row>
-    <row r="8" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A8" s="14">
         <v>3184</v>
       </c>
@@ -1846,7 +1846,7 @@
       <c r="BD8" s="2"/>
       <c r="BE8" s="2"/>
     </row>
-    <row r="9" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="9">
         <v>4408</v>
       </c>
@@ -1919,7 +1919,7 @@
       <c r="BD9" s="2"/>
       <c r="BE9" s="2"/>
     </row>
-    <row r="10" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="9">
         <v>6145</v>
       </c>
@@ -1990,7 +1990,7 @@
       <c r="BD10" s="2"/>
       <c r="BE10" s="2"/>
     </row>
-    <row r="11" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A11" s="9">
         <v>7475</v>
       </c>
@@ -2062,7 +2062,7 @@
       <c r="BD11" s="2"/>
       <c r="BE11" s="2"/>
     </row>
-    <row r="12" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
         <v>28</v>
       </c>
@@ -2134,7 +2134,7 @@
       <c r="BD12" s="2"/>
       <c r="BE12" s="2"/>
     </row>
-    <row r="13" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="7">
         <v>9961</v>
       </c>
@@ -2207,7 +2207,7 @@
       <c r="BD13" s="2"/>
       <c r="BE13" s="2"/>
     </row>
-    <row r="14" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A14" s="7">
         <v>9974</v>
       </c>
@@ -2278,7 +2278,7 @@
       <c r="BD14" s="2"/>
       <c r="BE14" s="2"/>
     </row>
-    <row r="15" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A15" s="7">
         <v>9974</v>
       </c>
@@ -2348,7 +2348,7 @@
       <c r="BD15" s="2"/>
       <c r="BE15" s="2"/>
     </row>
-    <row r="16" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A16" s="7">
         <v>9974</v>
       </c>
@@ -2420,7 +2420,7 @@
       <c r="BD16" s="2"/>
       <c r="BE16" s="2"/>
     </row>
-    <row r="17" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A17" s="7">
         <v>13743</v>
       </c>
@@ -2491,7 +2491,7 @@
       <c r="BD17" s="2"/>
       <c r="BE17" s="2"/>
     </row>
-    <row r="18" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A18" s="7">
         <v>16045</v>
       </c>
@@ -2561,7 +2561,7 @@
       <c r="BD18" s="2"/>
       <c r="BE18" s="2"/>
     </row>
-    <row r="19" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A19" s="7">
         <v>16356</v>
       </c>
@@ -2633,7 +2633,7 @@
       <c r="BD19" s="2"/>
       <c r="BE19" s="2"/>
     </row>
-    <row r="20" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A20" s="7">
         <v>16359</v>
       </c>
@@ -2703,7 +2703,7 @@
       <c r="BD20" s="2"/>
       <c r="BE20" s="2"/>
     </row>
-    <row r="21" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
         <v>38</v>
       </c>
@@ -2776,7 +2776,7 @@
       <c r="BD21" s="2"/>
       <c r="BE21" s="2"/>
     </row>
-    <row r="22" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
         <v>38</v>
       </c>
@@ -2849,7 +2849,7 @@
       <c r="BD22" s="2"/>
       <c r="BE22" s="2"/>
     </row>
-    <row r="23" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A23" s="7">
         <v>56362</v>
       </c>
@@ -2921,7 +2921,7 @@
       <c r="BD23" s="2"/>
       <c r="BE23" s="2"/>
     </row>
-    <row r="24" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="7"/>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -2980,15 +2980,15 @@
       <c r="BD24" s="2"/>
       <c r="BE24" s="2"/>
     </row>
-    <row r="25" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="7"/>
       <c r="J25" s="5"/>
     </row>
-    <row r="26" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="7"/>
       <c r="J26" s="5"/>
     </row>
-    <row r="27" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="7"/>
       <c r="B27" s="2"/>
       <c r="C27" s="2"/>
@@ -3047,7 +3047,7 @@
       <c r="BD27" s="2"/>
       <c r="BE27" s="2"/>
     </row>
-    <row r="28" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A28" s="7"/>
       <c r="B28" s="2"/>
       <c r="C28" s="2"/>
@@ -3105,15 +3105,15 @@
       <c r="BD28" s="2"/>
       <c r="BE28" s="2"/>
     </row>
-    <row r="29" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="7"/>
       <c r="J29" s="5"/>
     </row>
-    <row r="30" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:57" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="7"/>
       <c r="J30" s="5"/>
     </row>
-    <row r="31" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="7"/>
       <c r="B31" s="2"/>
       <c r="C31" s="2"/>
@@ -3172,7 +3172,7 @@
       <c r="BD31" s="2"/>
       <c r="BE31" s="2"/>
     </row>
-    <row r="32" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="7"/>
       <c r="B32" s="2"/>
       <c r="C32" s="2"/>
@@ -3231,7 +3231,7 @@
       <c r="BD32" s="2"/>
       <c r="BE32" s="2"/>
     </row>
-    <row r="33" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A33" s="7"/>
       <c r="B33" s="2"/>
       <c r="C33" s="2"/>
@@ -3289,7 +3289,7 @@
       <c r="BD33" s="2"/>
       <c r="BE33" s="2"/>
     </row>
-    <row r="34" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A34" s="7"/>
       <c r="B34" s="2"/>
       <c r="C34" s="2"/>
@@ -3347,7 +3347,7 @@
       <c r="BD34" s="2"/>
       <c r="BE34" s="2"/>
     </row>
-    <row r="35" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="7"/>
       <c r="B35" s="2"/>
       <c r="C35" s="2"/>
@@ -3406,7 +3406,7 @@
       <c r="BD35" s="2"/>
       <c r="BE35" s="2"/>
     </row>
-    <row r="36" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A36" s="7"/>
       <c r="B36" s="2"/>
       <c r="C36" s="2"/>
@@ -3464,7 +3464,7 @@
       <c r="BD36" s="2"/>
       <c r="BE36" s="2"/>
     </row>
-    <row r="37" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="7"/>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -3523,7 +3523,7 @@
       <c r="BD37" s="2"/>
       <c r="BE37" s="2"/>
     </row>
-    <row r="38" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="7"/>
       <c r="B38" s="2"/>
       <c r="C38" s="2"/>
@@ -3582,7 +3582,7 @@
       <c r="BD38" s="2"/>
       <c r="BE38" s="2"/>
     </row>
-    <row r="39" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="7"/>
       <c r="B39" s="2"/>
       <c r="C39" s="2"/>
@@ -3641,7 +3641,7 @@
       <c r="BD39" s="2"/>
       <c r="BE39" s="2"/>
     </row>
-    <row r="40" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A40" s="7"/>
       <c r="B40" s="2"/>
       <c r="C40" s="2"/>
@@ -3699,7 +3699,7 @@
       <c r="BD40" s="2"/>
       <c r="BE40" s="2"/>
     </row>
-    <row r="41" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="7"/>
       <c r="B41" s="2"/>
       <c r="C41" s="2"/>
@@ -3758,7 +3758,7 @@
       <c r="BD41" s="2"/>
       <c r="BE41" s="2"/>
     </row>
-    <row r="42" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="7"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
@@ -3817,7 +3817,7 @@
       <c r="BD42" s="2"/>
       <c r="BE42" s="2"/>
     </row>
-    <row r="43" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A43" s="7"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -3875,7 +3875,7 @@
       <c r="BD43" s="2"/>
       <c r="BE43" s="2"/>
     </row>
-    <row r="44" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A44" s="7"/>
       <c r="B44" s="2"/>
       <c r="C44" s="2"/>
@@ -3933,7 +3933,7 @@
       <c r="BD44" s="2"/>
       <c r="BE44" s="2"/>
     </row>
-    <row r="45" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A45" s="7"/>
       <c r="B45" s="2"/>
       <c r="C45" s="2"/>
@@ -3991,7 +3991,7 @@
       <c r="BD45" s="2"/>
       <c r="BE45" s="2"/>
     </row>
-    <row r="46" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A46" s="7"/>
       <c r="B46" s="2"/>
       <c r="C46" s="2"/>
@@ -4050,7 +4050,7 @@
       <c r="BD46" s="2"/>
       <c r="BE46" s="2"/>
     </row>
-    <row r="47" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A47" s="7"/>
       <c r="B47" s="2"/>
       <c r="C47" s="2"/>
@@ -4108,7 +4108,7 @@
       <c r="BD47" s="2"/>
       <c r="BE47" s="2"/>
     </row>
-    <row r="48" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A48" s="7"/>
       <c r="B48" s="2"/>
       <c r="C48" s="2"/>
@@ -4166,7 +4166,7 @@
       <c r="BD48" s="2"/>
       <c r="BE48" s="2"/>
     </row>
-    <row r="49" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A49" s="7"/>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -4224,7 +4224,7 @@
       <c r="BD49" s="2"/>
       <c r="BE49" s="2"/>
     </row>
-    <row r="50" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
       <c r="B50" s="2"/>
       <c r="C50" s="2"/>
@@ -4283,7 +4283,7 @@
       <c r="BD50" s="2"/>
       <c r="BE50" s="2"/>
     </row>
-    <row r="51" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
       <c r="B51" s="2"/>
       <c r="C51" s="2"/>
@@ -4342,7 +4342,7 @@
       <c r="BD51" s="2"/>
       <c r="BE51" s="2"/>
     </row>
-    <row r="52" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="7"/>
       <c r="B52" s="2"/>
       <c r="C52" s="2"/>
@@ -4401,7 +4401,7 @@
       <c r="BD52" s="2"/>
       <c r="BE52" s="2"/>
     </row>
-    <row r="53" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A53" s="7"/>
       <c r="B53" s="2"/>
       <c r="C53" s="2"/>
@@ -4459,7 +4459,7 @@
       <c r="BD53" s="2"/>
       <c r="BE53" s="2"/>
     </row>
-    <row r="54" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A54" s="7"/>
       <c r="B54" s="2"/>
       <c r="C54" s="2"/>
@@ -4517,7 +4517,7 @@
       <c r="BD54" s="2"/>
       <c r="BE54" s="2"/>
     </row>
-    <row r="55" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A55" s="7"/>
       <c r="B55" s="2"/>
       <c r="C55" s="2"/>
@@ -4576,7 +4576,7 @@
       <c r="BD55" s="2"/>
       <c r="BE55" s="2"/>
     </row>
-    <row r="56" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
       <c r="B56" s="2"/>
       <c r="C56" s="2"/>
@@ -4635,7 +4635,7 @@
       <c r="BD56" s="2"/>
       <c r="BE56" s="2"/>
     </row>
-    <row r="57" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
       <c r="B57" s="2"/>
       <c r="C57" s="2"/>
@@ -4693,7 +4693,7 @@
       <c r="BD57" s="2"/>
       <c r="BE57" s="2"/>
     </row>
-    <row r="58" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
       <c r="B58" s="2"/>
       <c r="C58" s="2"/>
@@ -4751,7 +4751,7 @@
       <c r="BD58" s="2"/>
       <c r="BE58" s="2"/>
     </row>
-    <row r="59" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A59" s="7"/>
       <c r="B59" s="2"/>
       <c r="C59" s="2"/>
@@ -4809,7 +4809,7 @@
       <c r="BD59" s="2"/>
       <c r="BE59" s="2"/>
     </row>
-    <row r="60" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -4868,7 +4868,7 @@
       <c r="BD60" s="2"/>
       <c r="BE60" s="2"/>
     </row>
-    <row r="61" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="7"/>
       <c r="B61" s="2"/>
       <c r="C61" s="2"/>
@@ -4927,7 +4927,7 @@
       <c r="BD61" s="2"/>
       <c r="BE61" s="2"/>
     </row>
-    <row r="62" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
       <c r="B62" s="2"/>
       <c r="C62" s="2"/>
@@ -4986,7 +4986,7 @@
       <c r="BD62" s="2"/>
       <c r="BE62" s="2"/>
     </row>
-    <row r="63" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A63" s="8"/>
       <c r="B63" s="2"/>
       <c r="C63" s="2"/>
@@ -5044,7 +5044,7 @@
       <c r="BD63" s="2"/>
       <c r="BE63" s="2"/>
     </row>
-    <row r="64" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="8"/>
       <c r="B64" s="2"/>
       <c r="C64" s="2"/>
@@ -5103,7 +5103,7 @@
       <c r="BD64" s="2"/>
       <c r="BE64" s="2"/>
     </row>
-    <row r="65" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="8"/>
       <c r="B65" s="2"/>
       <c r="C65" s="2"/>
@@ -5162,7 +5162,7 @@
       <c r="BD65" s="2"/>
       <c r="BE65" s="2"/>
     </row>
-    <row r="66" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A66" s="16"/>
       <c r="B66" s="2"/>
       <c r="C66" s="2"/>
@@ -5220,7 +5220,7 @@
       <c r="BD66" s="2"/>
       <c r="BE66" s="2"/>
     </row>
-    <row r="67" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="16"/>
       <c r="B67" s="2"/>
       <c r="C67" s="2"/>
@@ -5279,7 +5279,7 @@
       <c r="BD67" s="2"/>
       <c r="BE67" s="2"/>
     </row>
-    <row r="68" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A68" s="7"/>
       <c r="B68" s="2"/>
       <c r="C68" s="2"/>
@@ -5337,7 +5337,7 @@
       <c r="BD68" s="2"/>
       <c r="BE68" s="2"/>
     </row>
-    <row r="69" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
       <c r="B69" s="2"/>
       <c r="C69" s="2"/>
@@ -5396,7 +5396,7 @@
       <c r="BD69" s="2"/>
       <c r="BE69" s="2"/>
     </row>
-    <row r="70" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="7"/>
       <c r="B70" s="2"/>
       <c r="C70" s="2"/>
@@ -5455,7 +5455,7 @@
       <c r="BD70" s="2"/>
       <c r="BE70" s="2"/>
     </row>
-    <row r="71" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A71" s="7"/>
       <c r="B71" s="2"/>
       <c r="C71" s="2"/>
@@ -5513,7 +5513,7 @@
       <c r="BD71" s="2"/>
       <c r="BE71" s="2"/>
     </row>
-    <row r="72" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A72" s="7"/>
       <c r="B72" s="2"/>
       <c r="C72" s="2"/>
@@ -5571,7 +5571,7 @@
       <c r="BD72" s="2"/>
       <c r="BE72" s="2"/>
     </row>
-    <row r="73" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="7"/>
       <c r="B73" s="2"/>
       <c r="C73" s="2"/>
@@ -5630,7 +5630,7 @@
       <c r="BD73" s="2"/>
       <c r="BE73" s="2"/>
     </row>
-    <row r="74" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="7"/>
       <c r="B74" s="2"/>
       <c r="C74" s="2"/>
@@ -5689,7 +5689,7 @@
       <c r="BD74" s="2"/>
       <c r="BE74" s="2"/>
     </row>
-    <row r="75" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A75" s="8"/>
       <c r="B75" s="3"/>
       <c r="C75" s="3"/>
@@ -5747,7 +5747,7 @@
       <c r="BD75" s="2"/>
       <c r="BE75" s="2"/>
     </row>
-    <row r="76" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
       <c r="B76" s="3"/>
       <c r="C76" s="3"/>
@@ -5805,7 +5805,7 @@
       <c r="BD76" s="2"/>
       <c r="BE76" s="2"/>
     </row>
-    <row r="77" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
       <c r="B77" s="3"/>
       <c r="C77" s="3"/>
@@ -5863,7 +5863,7 @@
       <c r="BD77" s="2"/>
       <c r="BE77" s="2"/>
     </row>
-    <row r="78" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
       <c r="B78" s="3"/>
       <c r="C78" s="3"/>
@@ -5922,7 +5922,7 @@
       <c r="BD78" s="2"/>
       <c r="BE78" s="2"/>
     </row>
-    <row r="79" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A79" s="8"/>
       <c r="B79" s="3"/>
       <c r="C79" s="3"/>
@@ -5981,7 +5981,7 @@
       <c r="BD79" s="2"/>
       <c r="BE79" s="2"/>
     </row>
-    <row r="80" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A80" s="8"/>
       <c r="B80" s="3"/>
       <c r="C80" s="3"/>
@@ -6039,7 +6039,7 @@
       <c r="BD80" s="2"/>
       <c r="BE80" s="2"/>
     </row>
-    <row r="81" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A81" s="8"/>
       <c r="B81" s="3"/>
       <c r="C81" s="3"/>
@@ -6097,7 +6097,7 @@
       <c r="BD81" s="2"/>
       <c r="BE81" s="2"/>
     </row>
-    <row r="82" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A82" s="8"/>
       <c r="B82" s="3"/>
       <c r="C82" s="3"/>
@@ -6156,7 +6156,7 @@
       <c r="BD82" s="2"/>
       <c r="BE82" s="2"/>
     </row>
-    <row r="83" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A83" s="8"/>
       <c r="B83" s="3"/>
       <c r="C83" s="3"/>
@@ -6215,7 +6215,7 @@
       <c r="BD83" s="2"/>
       <c r="BE83" s="2"/>
     </row>
-    <row r="84" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A84" s="8"/>
       <c r="B84" s="3"/>
       <c r="C84" s="3"/>
@@ -6274,7 +6274,7 @@
       <c r="BD84" s="2"/>
       <c r="BE84" s="2"/>
     </row>
-    <row r="85" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A85" s="8"/>
       <c r="B85" s="3"/>
       <c r="C85" s="3"/>
@@ -6332,7 +6332,7 @@
       <c r="BD85" s="2"/>
       <c r="BE85" s="2"/>
     </row>
-    <row r="86" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A86" s="8"/>
       <c r="B86" s="3"/>
       <c r="C86" s="3"/>
@@ -6390,7 +6390,7 @@
       <c r="BD86" s="2"/>
       <c r="BE86" s="2"/>
     </row>
-    <row r="87" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A87" s="8"/>
       <c r="B87" s="3"/>
       <c r="C87" s="3"/>
@@ -6449,7 +6449,7 @@
       <c r="BD87" s="2"/>
       <c r="BE87" s="2"/>
     </row>
-    <row r="88" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A88" s="8"/>
       <c r="B88" s="3"/>
       <c r="C88" s="3"/>
@@ -6507,7 +6507,7 @@
       <c r="BD88" s="2"/>
       <c r="BE88" s="2"/>
     </row>
-    <row r="89" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A89" s="8"/>
       <c r="B89" s="3"/>
       <c r="C89" s="3"/>
@@ -6565,7 +6565,7 @@
       <c r="BD89" s="2"/>
       <c r="BE89" s="2"/>
     </row>
-    <row r="90" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A90" s="8"/>
       <c r="B90" s="3"/>
       <c r="C90" s="3"/>
@@ -6624,7 +6624,7 @@
       <c r="BD90" s="2"/>
       <c r="BE90" s="2"/>
     </row>
-    <row r="91" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A91" s="8"/>
       <c r="B91" s="3"/>
       <c r="C91" s="3"/>
@@ -6683,7 +6683,7 @@
       <c r="BD91" s="2"/>
       <c r="BE91" s="2"/>
     </row>
-    <row r="92" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A92" s="8"/>
       <c r="B92" s="3"/>
       <c r="C92" s="3"/>
@@ -6741,7 +6741,7 @@
       <c r="BD92" s="2"/>
       <c r="BE92" s="2"/>
     </row>
-    <row r="93" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A93" s="8"/>
       <c r="B93" s="3"/>
       <c r="C93" s="3"/>
@@ -6799,7 +6799,7 @@
       <c r="BD93" s="2"/>
       <c r="BE93" s="2"/>
     </row>
-    <row r="94" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A94" s="8"/>
       <c r="B94" s="3"/>
       <c r="C94" s="3"/>
@@ -6858,7 +6858,7 @@
       <c r="BD94" s="2"/>
       <c r="BE94" s="2"/>
     </row>
-    <row r="95" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A95" s="7"/>
       <c r="B95" s="3"/>
       <c r="C95" s="3"/>
@@ -6916,7 +6916,7 @@
       <c r="BD95" s="2"/>
       <c r="BE95" s="2"/>
     </row>
-    <row r="96" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A96" s="8"/>
       <c r="B96" s="3"/>
       <c r="C96" s="3"/>
@@ -6974,7 +6974,7 @@
       <c r="BD96" s="2"/>
       <c r="BE96" s="2"/>
     </row>
-    <row r="97" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A97" s="8"/>
       <c r="B97" s="3"/>
       <c r="C97" s="3"/>
@@ -7032,7 +7032,7 @@
       <c r="BD97" s="2"/>
       <c r="BE97" s="2"/>
     </row>
-    <row r="98" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8"/>
       <c r="B98" s="3"/>
       <c r="C98" s="3"/>
@@ -7091,7 +7091,7 @@
       <c r="BD98" s="2"/>
       <c r="BE98" s="2"/>
     </row>
-    <row r="99" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A99" s="8"/>
       <c r="B99" s="3"/>
       <c r="C99" s="3"/>
@@ -7149,7 +7149,7 @@
       <c r="BD99" s="2"/>
       <c r="BE99" s="2"/>
     </row>
-    <row r="100" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A100" s="8"/>
       <c r="B100" s="3"/>
       <c r="C100" s="3"/>
@@ -7208,7 +7208,7 @@
       <c r="BD100" s="2"/>
       <c r="BE100" s="2"/>
     </row>
-    <row r="101" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A101" s="8"/>
       <c r="B101" s="3"/>
       <c r="C101" s="3"/>
@@ -7266,7 +7266,7 @@
       <c r="BD101" s="2"/>
       <c r="BE101" s="2"/>
     </row>
-    <row r="102" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A102" s="7"/>
       <c r="B102" s="3"/>
       <c r="C102" s="3"/>
@@ -7324,7 +7324,7 @@
       <c r="BD102" s="2"/>
       <c r="BE102" s="2"/>
     </row>
-    <row r="103" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A103" s="8"/>
       <c r="B103" s="3"/>
       <c r="C103" s="3"/>
@@ -7383,7 +7383,7 @@
       <c r="BD103" s="2"/>
       <c r="BE103" s="2"/>
     </row>
-    <row r="104" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A104" s="8"/>
       <c r="B104" s="3"/>
       <c r="C104" s="3"/>
@@ -7442,7 +7442,7 @@
       <c r="BD104" s="2"/>
       <c r="BE104" s="2"/>
     </row>
-    <row r="105" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A105" s="7"/>
       <c r="B105" s="3"/>
       <c r="C105" s="3"/>
@@ -7500,7 +7500,7 @@
       <c r="BD105" s="2"/>
       <c r="BE105" s="2"/>
     </row>
-    <row r="106" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A106" s="7"/>
       <c r="B106" s="3"/>
       <c r="C106" s="3"/>
@@ -7558,7 +7558,7 @@
       <c r="BD106" s="2"/>
       <c r="BE106" s="2"/>
     </row>
-    <row r="107" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A107" s="7"/>
       <c r="B107" s="3"/>
       <c r="C107" s="3"/>
@@ -7617,7 +7617,7 @@
       <c r="BD107" s="2"/>
       <c r="BE107" s="2"/>
     </row>
-    <row r="108" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:57" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A108" s="7"/>
       <c r="B108" s="3"/>
       <c r="C108" s="3"/>
@@ -7676,7 +7676,7 @@
       <c r="BD108" s="2"/>
       <c r="BE108" s="2"/>
     </row>
-    <row r="109" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A109" s="7"/>
       <c r="B109" s="3"/>
       <c r="C109" s="3"/>
@@ -7734,170 +7734,170 @@
       <c r="BD109" s="2"/>
       <c r="BE109" s="2"/>
     </row>
-    <row r="110" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A110" s="7"/>
       <c r="I110" s="3"/>
       <c r="K110" s="3"/>
       <c r="L110" s="3"/>
       <c r="N110" s="2"/>
     </row>
-    <row r="111" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:57" x14ac:dyDescent="0.25">
       <c r="A111" s="7"/>
       <c r="I111" s="3"/>
       <c r="K111" s="3"/>
       <c r="L111" s="3"/>
       <c r="N111" s="2"/>
     </row>
-    <row r="112" spans="1:57" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:57" x14ac:dyDescent="0.25">
       <c r="I112" s="3"/>
       <c r="K112" s="3"/>
       <c r="L112" s="10"/>
       <c r="N112" s="2"/>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113" s="7"/>
       <c r="I113" s="3"/>
       <c r="K113" s="3"/>
       <c r="L113" s="3"/>
       <c r="N113" s="2"/>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114" s="7"/>
       <c r="I114" s="3"/>
       <c r="K114" s="3"/>
       <c r="L114" s="3"/>
       <c r="N114" s="2"/>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115" s="7"/>
       <c r="I115" s="3"/>
       <c r="K115" s="3"/>
       <c r="L115" s="3"/>
       <c r="N115" s="2"/>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116" s="7"/>
       <c r="I116" s="3"/>
       <c r="K116" s="3"/>
       <c r="L116" s="3"/>
       <c r="N116" s="2"/>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117" s="7"/>
       <c r="I117" s="3"/>
       <c r="K117" s="3"/>
       <c r="L117" s="3"/>
       <c r="N117" s="2"/>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I118" s="3"/>
       <c r="K118" s="3"/>
       <c r="L118" s="3"/>
       <c r="N118" s="2"/>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119" s="7"/>
       <c r="I119" s="3"/>
       <c r="K119" s="3"/>
       <c r="L119" s="3"/>
       <c r="N119" s="2"/>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120" s="7"/>
       <c r="I120" s="3"/>
       <c r="K120" s="3"/>
       <c r="L120" s="3"/>
       <c r="N120" s="2"/>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121" s="7"/>
       <c r="I121" s="3"/>
       <c r="K121" s="3"/>
       <c r="L121" s="3"/>
       <c r="N121" s="2"/>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I122" s="3"/>
       <c r="K122" s="3"/>
       <c r="L122" s="3"/>
       <c r="N122" s="2"/>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I123" s="3"/>
       <c r="K123" s="3"/>
       <c r="L123" s="3"/>
       <c r="N123" s="2"/>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I124" s="3"/>
       <c r="K124" s="3"/>
       <c r="L124" s="3"/>
       <c r="N124" s="2"/>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I125" s="3"/>
       <c r="K125" s="3"/>
       <c r="L125" s="3"/>
       <c r="N125" s="2"/>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I126" s="3"/>
       <c r="K126" s="3"/>
       <c r="L126" s="3"/>
       <c r="N126" s="2"/>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I127" s="3"/>
       <c r="K127" s="3"/>
       <c r="L127" s="3"/>
       <c r="N127" s="2"/>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I128" s="3"/>
       <c r="K128" s="3"/>
       <c r="L128" s="3"/>
       <c r="N128" s="2"/>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I129" s="3"/>
       <c r="K129" s="3"/>
       <c r="L129" s="3"/>
       <c r="N129" s="2"/>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I130" s="3"/>
       <c r="K130" s="3"/>
       <c r="L130" s="3"/>
       <c r="N130" s="2"/>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I131" s="3"/>
       <c r="K131" s="3"/>
       <c r="L131" s="3"/>
       <c r="N131" s="2"/>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132" s="7"/>
       <c r="I132" s="3"/>
       <c r="K132" s="3"/>
       <c r="L132" s="3"/>
       <c r="N132" s="2"/>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133" s="7"/>
       <c r="I133" s="3"/>
       <c r="K133" s="3"/>
       <c r="L133" s="3"/>
       <c r="N133" s="2"/>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134" s="7"/>
       <c r="I134" s="3"/>
       <c r="K134" s="3"/>
       <c r="L134" s="3"/>
       <c r="N134" s="2"/>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135" s="7"/>
       <c r="I135" s="3"/>
       <c r="J135" s="5"/>
@@ -7905,172 +7905,172 @@
       <c r="L135" s="3"/>
       <c r="N135" s="2"/>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136" s="7"/>
       <c r="I136" s="3"/>
       <c r="K136" s="3"/>
       <c r="L136" s="3"/>
       <c r="N136" s="2"/>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137" s="7"/>
       <c r="I137" s="3"/>
       <c r="K137" s="3"/>
       <c r="L137" s="3"/>
       <c r="N137" s="2"/>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138" s="7"/>
       <c r="I138" s="3"/>
       <c r="K138" s="3"/>
       <c r="L138" s="3"/>
       <c r="N138" s="2"/>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139" s="7"/>
       <c r="I139" s="3"/>
       <c r="K139" s="3"/>
       <c r="L139" s="3"/>
       <c r="N139" s="2"/>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140" s="7"/>
       <c r="I140" s="3"/>
       <c r="K140" s="3"/>
       <c r="L140" s="3"/>
       <c r="N140" s="2"/>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141" s="7"/>
       <c r="I141" s="3"/>
       <c r="K141" s="3"/>
       <c r="L141" s="3"/>
       <c r="N141" s="2"/>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142" s="7"/>
       <c r="I142" s="3"/>
       <c r="K142" s="3"/>
       <c r="L142" s="3"/>
       <c r="N142" s="2"/>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143" s="7"/>
       <c r="I143" s="3"/>
       <c r="K143" s="3"/>
       <c r="L143" s="3"/>
       <c r="N143" s="2"/>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144" s="7"/>
       <c r="I144" s="3"/>
       <c r="K144" s="3"/>
       <c r="L144" s="3"/>
       <c r="N144" s="2"/>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I145" s="3"/>
       <c r="K145" s="3"/>
       <c r="L145" s="3"/>
       <c r="N145" s="2"/>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I146" s="3"/>
       <c r="K146" s="3"/>
       <c r="L146" s="3"/>
       <c r="N146" s="2"/>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I147" s="3"/>
       <c r="K147" s="3"/>
       <c r="L147" s="3"/>
       <c r="N147" s="2"/>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I148" s="3"/>
       <c r="K148" s="3"/>
       <c r="L148" s="3"/>
       <c r="N148" s="2"/>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I149" s="3"/>
       <c r="K149" s="3"/>
       <c r="L149" s="3"/>
       <c r="N149" s="2"/>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I150" s="3"/>
       <c r="K150" s="3"/>
       <c r="L150" s="3"/>
       <c r="N150" s="2"/>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I151" s="3"/>
       <c r="K151" s="3"/>
       <c r="L151" s="3"/>
       <c r="N151" s="2"/>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I152" s="3"/>
       <c r="K152" s="3"/>
       <c r="L152" s="3"/>
       <c r="N152" s="2"/>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I153" s="3"/>
       <c r="K153" s="3"/>
       <c r="L153" s="3"/>
       <c r="N153" s="2"/>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154" s="7"/>
       <c r="I154" s="3"/>
       <c r="K154" s="3"/>
       <c r="L154" s="3"/>
       <c r="N154" s="2"/>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155" s="7"/>
       <c r="I155" s="3"/>
       <c r="K155" s="3"/>
       <c r="L155" s="3"/>
       <c r="N155" s="2"/>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I156" s="3"/>
       <c r="K156" s="3"/>
       <c r="L156" s="3"/>
       <c r="N156" s="2"/>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I157" s="3"/>
       <c r="K157" s="3"/>
       <c r="L157" s="3"/>
       <c r="N157" s="2"/>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I158" s="3"/>
       <c r="K158" s="3"/>
       <c r="L158" s="3"/>
       <c r="N158" s="2"/>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I159" s="3"/>
       <c r="K159" s="3"/>
       <c r="L159" s="10"/>
       <c r="N159" s="2"/>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I160" s="3"/>
       <c r="K160" s="3"/>
       <c r="N160" s="2"/>
     </row>
-    <row r="161" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I161" s="3"/>
       <c r="K161" s="3"/>
       <c r="N161" s="2"/>
     </row>
-    <row r="162" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="B162" s="9"/>
       <c r="C162" s="9"/>
       <c r="D162" s="9"/>
@@ -8082,57 +8082,57 @@
       <c r="K162" s="3"/>
       <c r="N162" s="2"/>
     </row>
-    <row r="163" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I163" s="3"/>
       <c r="K163" s="3"/>
       <c r="N163" s="2"/>
     </row>
-    <row r="164" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I164" s="3"/>
       <c r="K164" s="3"/>
       <c r="L164" s="3"/>
       <c r="N164" s="2"/>
     </row>
-    <row r="165" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="7"/>
       <c r="I165" s="3"/>
       <c r="K165" s="6"/>
       <c r="L165" s="10"/>
       <c r="N165" s="2"/>
     </row>
-    <row r="166" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="7"/>
       <c r="I166" s="3"/>
       <c r="K166" s="3"/>
       <c r="L166" s="3"/>
       <c r="N166" s="2"/>
     </row>
-    <row r="167" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="7"/>
       <c r="I167" s="3"/>
       <c r="K167" s="3"/>
       <c r="L167" s="3"/>
       <c r="N167" s="2"/>
     </row>
-    <row r="168" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I168" s="3"/>
       <c r="K168" s="3"/>
       <c r="L168" s="3"/>
       <c r="N168" s="2"/>
     </row>
-    <row r="169" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I169" s="3"/>
       <c r="K169" s="3"/>
       <c r="L169" s="3"/>
       <c r="N169" s="2"/>
     </row>
-    <row r="170" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I170" s="3"/>
       <c r="K170" s="3"/>
       <c r="L170" s="3"/>
       <c r="N170" s="2"/>
     </row>
-    <row r="171" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="7"/>
       <c r="I171" s="3"/>
       <c r="K171" s="3"/>
@@ -8141,34 +8141,34 @@
       <c r="N171" s="2"/>
       <c r="P171" s="2"/>
     </row>
-    <row r="172" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="7"/>
       <c r="I172" s="3"/>
       <c r="K172" s="3"/>
       <c r="N172" s="2"/>
     </row>
-    <row r="173" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="7"/>
       <c r="I173" s="3"/>
       <c r="K173" s="3"/>
       <c r="L173" s="3"/>
       <c r="N173" s="2"/>
     </row>
-    <row r="174" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="7"/>
       <c r="I174" s="3"/>
       <c r="K174" s="3"/>
       <c r="L174" s="3"/>
       <c r="N174" s="2"/>
     </row>
-    <row r="175" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="7"/>
       <c r="I175" s="3"/>
       <c r="K175" s="3"/>
       <c r="L175" s="3"/>
       <c r="N175" s="2"/>
     </row>
-    <row r="176" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="7"/>
       <c r="I176" s="3"/>
       <c r="K176" s="10"/>
@@ -8176,184 +8176,184 @@
       <c r="M176" s="10"/>
       <c r="N176" s="2"/>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177" s="7"/>
       <c r="I177" s="3"/>
       <c r="K177" s="3"/>
       <c r="L177" s="3"/>
       <c r="N177" s="2"/>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178" s="7"/>
       <c r="I178" s="3"/>
       <c r="K178" s="3"/>
       <c r="L178" s="3"/>
       <c r="N178" s="2"/>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179" s="7"/>
       <c r="I179" s="3"/>
       <c r="K179" s="3"/>
       <c r="L179" s="3"/>
       <c r="N179" s="2"/>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180" s="7"/>
       <c r="I180" s="3"/>
       <c r="K180" s="3"/>
       <c r="L180" s="3"/>
       <c r="N180" s="2"/>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181" s="7"/>
       <c r="I181" s="3"/>
       <c r="K181" s="3"/>
       <c r="L181" s="3"/>
       <c r="N181" s="2"/>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182" s="7"/>
       <c r="I182" s="3"/>
       <c r="K182" s="3"/>
       <c r="L182" s="3"/>
       <c r="N182" s="2"/>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183" s="7"/>
       <c r="I183" s="3"/>
       <c r="K183" s="3"/>
       <c r="L183" s="3"/>
       <c r="N183" s="2"/>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184" s="7"/>
       <c r="I184" s="3"/>
       <c r="K184" s="3"/>
       <c r="L184" s="3"/>
       <c r="N184" s="2"/>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185" s="7"/>
       <c r="I185" s="3"/>
       <c r="K185" s="3"/>
       <c r="L185" s="3"/>
       <c r="N185" s="2"/>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186" s="7"/>
       <c r="I186" s="3"/>
       <c r="K186" s="3"/>
       <c r="L186" s="3"/>
       <c r="N186" s="2"/>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187" s="7"/>
       <c r="I187" s="3"/>
       <c r="K187" s="3"/>
       <c r="L187" s="3"/>
       <c r="N187" s="2"/>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188" s="7"/>
       <c r="I188" s="3"/>
       <c r="K188" s="3"/>
       <c r="L188" s="3"/>
       <c r="N188" s="2"/>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I189" s="3"/>
       <c r="K189" s="3"/>
       <c r="L189" s="3"/>
       <c r="N189" s="2"/>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190" s="7"/>
       <c r="I190" s="3"/>
       <c r="K190" s="3"/>
       <c r="L190" s="3"/>
       <c r="N190" s="2"/>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A191" s="7"/>
       <c r="I191" s="3"/>
       <c r="K191" s="3"/>
       <c r="L191" s="3"/>
       <c r="N191" s="2"/>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192" s="7"/>
       <c r="I192" s="3"/>
       <c r="K192" s="3"/>
       <c r="L192" s="3"/>
       <c r="N192" s="2"/>
     </row>
-    <row r="193" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="193" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A193" s="7"/>
       <c r="I193" s="3"/>
       <c r="K193" s="3"/>
       <c r="L193" s="3"/>
       <c r="N193" s="2"/>
     </row>
-    <row r="194" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="194" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A194" s="7"/>
       <c r="I194" s="3"/>
       <c r="K194" s="3"/>
       <c r="L194" s="10"/>
       <c r="N194" s="2"/>
     </row>
-    <row r="195" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="195" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A195" s="7"/>
       <c r="I195" s="3"/>
       <c r="K195" s="3"/>
       <c r="L195" s="3"/>
       <c r="N195" s="2"/>
     </row>
-    <row r="196" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="196" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A196" s="7"/>
       <c r="I196" s="3"/>
       <c r="K196" s="3"/>
       <c r="L196" s="10"/>
       <c r="N196" s="2"/>
     </row>
-    <row r="197" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="197" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A197" s="7"/>
       <c r="I197" s="3"/>
       <c r="K197" s="3"/>
       <c r="L197" s="10"/>
       <c r="N197" s="2"/>
     </row>
-    <row r="198" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="198" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A198" s="7"/>
       <c r="I198" s="3"/>
       <c r="K198" s="3"/>
       <c r="L198" s="3"/>
       <c r="N198" s="2"/>
     </row>
-    <row r="199" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="199" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I199" s="3"/>
       <c r="K199" s="3"/>
       <c r="L199" s="3"/>
       <c r="N199" s="2"/>
     </row>
-    <row r="200" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="200" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I200" s="3"/>
       <c r="K200" s="3"/>
       <c r="L200" s="10"/>
       <c r="N200" s="2"/>
     </row>
-    <row r="201" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="201" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A201" s="7"/>
       <c r="I201" s="3"/>
       <c r="K201" s="3"/>
       <c r="N201" s="2"/>
     </row>
-    <row r="202" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="202" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A202" s="7"/>
       <c r="I202" s="3"/>
       <c r="K202" s="11"/>
       <c r="N202" s="2"/>
     </row>
-    <row r="203" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="203" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A203" s="7"/>
       <c r="I203" s="3"/>
       <c r="K203" s="11"/>
@@ -8361,597 +8361,597 @@
       <c r="N203" s="2"/>
       <c r="P203" s="7"/>
     </row>
-    <row r="204" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="204" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A204" s="7"/>
       <c r="I204" s="3"/>
       <c r="K204" s="11"/>
       <c r="L204" s="11"/>
       <c r="N204" s="2"/>
     </row>
-    <row r="205" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="205" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A205" s="7"/>
       <c r="I205" s="3"/>
       <c r="K205" s="11"/>
       <c r="L205" s="11"/>
       <c r="N205" s="2"/>
     </row>
-    <row r="206" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="206" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A206" s="7"/>
       <c r="I206" s="3"/>
       <c r="K206" s="11"/>
       <c r="L206" s="11"/>
       <c r="N206" s="2"/>
     </row>
-    <row r="207" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="207" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I207" s="3"/>
       <c r="K207" s="11"/>
       <c r="L207" s="11"/>
       <c r="N207" s="2"/>
     </row>
-    <row r="208" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="208" spans="1:16" x14ac:dyDescent="0.25">
       <c r="I208" s="3"/>
       <c r="K208" s="11"/>
       <c r="L208" s="11"/>
       <c r="N208" s="2"/>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I209" s="3"/>
       <c r="K209" s="11"/>
       <c r="L209" s="10"/>
       <c r="N209" s="2"/>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210" s="7"/>
       <c r="I210" s="3"/>
       <c r="K210" s="11"/>
       <c r="L210" s="11"/>
       <c r="N210" s="2"/>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211" s="7"/>
       <c r="I211" s="3"/>
       <c r="K211" s="11"/>
       <c r="L211" s="11"/>
       <c r="N211" s="2"/>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212" s="7"/>
       <c r="I212" s="3"/>
       <c r="K212" s="11"/>
       <c r="L212" s="11"/>
       <c r="N212" s="2"/>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213" s="7"/>
       <c r="I213" s="3"/>
       <c r="K213" s="11"/>
       <c r="L213" s="11"/>
       <c r="N213" s="2"/>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214" s="7"/>
       <c r="I214" s="3"/>
       <c r="K214" s="11"/>
       <c r="L214" s="11"/>
       <c r="N214" s="2"/>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215" s="7"/>
       <c r="I215" s="3"/>
       <c r="K215" s="11"/>
       <c r="L215" s="11"/>
       <c r="N215" s="2"/>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216" s="7"/>
       <c r="I216" s="3"/>
       <c r="K216" s="11"/>
       <c r="L216" s="11"/>
       <c r="N216" s="2"/>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217" s="7"/>
       <c r="I217" s="3"/>
       <c r="K217" s="11"/>
       <c r="L217" s="11"/>
       <c r="N217" s="2"/>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218" s="7"/>
       <c r="I218" s="3"/>
       <c r="K218" s="11"/>
       <c r="L218" s="11"/>
       <c r="N218" s="2"/>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A219" s="7"/>
       <c r="I219" s="3"/>
       <c r="K219" s="11"/>
       <c r="L219" s="11"/>
       <c r="N219" s="2"/>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220" s="7"/>
       <c r="I220" s="3"/>
       <c r="K220" s="11"/>
       <c r="L220" s="11"/>
       <c r="N220" s="2"/>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I221" s="3"/>
       <c r="K221" s="10"/>
       <c r="L221" s="11"/>
       <c r="N221" s="2"/>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I222" s="3"/>
       <c r="K222" s="11"/>
       <c r="L222" s="11"/>
       <c r="N222" s="2"/>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I223" s="3"/>
       <c r="K223" s="11"/>
       <c r="L223" s="11"/>
       <c r="N223" s="2"/>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224" s="7"/>
       <c r="I224" s="3"/>
       <c r="K224" s="11"/>
       <c r="L224" s="11"/>
       <c r="N224" s="2"/>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A225" s="7"/>
       <c r="I225" s="3"/>
       <c r="K225" s="11"/>
       <c r="L225" s="11"/>
       <c r="N225" s="2"/>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226" s="7"/>
       <c r="I226" s="3"/>
       <c r="K226" s="11"/>
       <c r="L226" s="11"/>
       <c r="N226" s="2"/>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227" s="7"/>
       <c r="I227" s="3"/>
       <c r="K227" s="11"/>
       <c r="L227" s="11"/>
       <c r="N227" s="2"/>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228" s="7"/>
       <c r="I228" s="3"/>
       <c r="K228" s="11"/>
       <c r="L228" s="11"/>
       <c r="N228" s="2"/>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229" s="7"/>
       <c r="I229" s="3"/>
       <c r="K229" s="11"/>
       <c r="L229" s="11"/>
       <c r="N229" s="2"/>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230" s="7"/>
       <c r="I230" s="3"/>
       <c r="K230" s="11"/>
       <c r="L230" s="11"/>
       <c r="N230" s="2"/>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231" s="7"/>
       <c r="I231" s="3"/>
       <c r="K231" s="11"/>
       <c r="L231" s="11"/>
       <c r="N231" s="2"/>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I232" s="3"/>
       <c r="K232" s="11"/>
       <c r="L232" s="11"/>
       <c r="N232" s="2"/>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A233" s="7"/>
       <c r="I233" s="3"/>
       <c r="K233" s="11"/>
       <c r="L233" s="11"/>
       <c r="N233" s="2"/>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234" s="7"/>
       <c r="I234" s="3"/>
       <c r="K234" s="11"/>
       <c r="L234" s="11"/>
       <c r="N234" s="2"/>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235" s="7"/>
       <c r="I235" s="3"/>
       <c r="N235" s="2"/>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236" s="7"/>
       <c r="I236" s="3"/>
       <c r="N236" s="2"/>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237" s="7"/>
       <c r="I237" s="3"/>
       <c r="N237" s="2"/>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A238" s="7"/>
       <c r="I238" s="3"/>
       <c r="N238" s="2"/>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I239" s="3"/>
       <c r="N239" s="2"/>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A240" s="7"/>
       <c r="I240" s="3"/>
       <c r="N240" s="2"/>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A241" s="7"/>
       <c r="N241" s="2"/>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A242" s="7"/>
       <c r="N242" s="2"/>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A243" s="7"/>
       <c r="N243" s="2"/>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A244" s="7"/>
       <c r="N244" s="2"/>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A245" s="7"/>
       <c r="N245" s="2"/>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A246" s="7"/>
       <c r="N246" s="2"/>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N247" s="2"/>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A248" s="7"/>
       <c r="N248" s="2"/>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A249" s="7"/>
       <c r="N249" s="2"/>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
       <c r="J250" s="12"/>
       <c r="N250" s="2"/>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N251" s="2"/>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N252" s="2"/>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A253" s="7"/>
       <c r="N253" s="2"/>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254" s="7"/>
       <c r="N254" s="2"/>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="N255" s="2"/>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256" s="7"/>
       <c r="K256" s="13"/>
       <c r="N256" s="2"/>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257" s="7"/>
       <c r="K257" s="11"/>
       <c r="N257" s="2"/>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A258" s="7"/>
       <c r="K258" s="11"/>
       <c r="L258" s="11"/>
       <c r="N258" s="2"/>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A259" s="7"/>
       <c r="K259" s="11"/>
       <c r="L259" s="11"/>
       <c r="N259" s="2"/>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A260" s="7"/>
       <c r="K260" s="11"/>
       <c r="L260" s="11"/>
       <c r="N260" s="2"/>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A261" s="7"/>
       <c r="K261" s="11"/>
       <c r="L261" s="11"/>
       <c r="N261" s="2"/>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A262" s="7"/>
       <c r="K262" s="11"/>
       <c r="L262" s="11"/>
       <c r="N262" s="2"/>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A263" s="7"/>
       <c r="K263" s="11"/>
       <c r="L263" s="11"/>
       <c r="N263" s="2"/>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A264" s="7"/>
       <c r="K264" s="11"/>
       <c r="L264" s="11"/>
       <c r="N264" s="2"/>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A265" s="7"/>
       <c r="K265" s="11"/>
       <c r="L265" s="11"/>
       <c r="N265" s="2"/>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A266" s="7"/>
       <c r="K266" s="11"/>
       <c r="L266" s="11"/>
       <c r="N266" s="2"/>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A267" s="7"/>
       <c r="K267" s="11"/>
       <c r="L267" s="11"/>
       <c r="N267" s="2"/>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A268" s="7"/>
       <c r="K268" s="11"/>
       <c r="L268" s="11"/>
       <c r="N268" s="2"/>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A269" s="7"/>
       <c r="K269" s="11"/>
       <c r="L269" s="11"/>
       <c r="N269" s="2"/>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K270" s="11"/>
       <c r="L270" s="11"/>
       <c r="N270" s="2"/>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K271" s="11"/>
       <c r="L271" s="11"/>
       <c r="N271" s="2"/>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K272" s="11"/>
       <c r="L272" s="11"/>
       <c r="N272" s="2"/>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A273" s="7"/>
       <c r="K273" s="11"/>
       <c r="L273" s="11"/>
       <c r="N273" s="2"/>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A274" s="7"/>
       <c r="K274" s="11"/>
       <c r="L274" s="11"/>
       <c r="N274" s="2"/>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A275" s="7"/>
       <c r="K275" s="11"/>
       <c r="L275" s="11"/>
       <c r="N275" s="2"/>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K276" s="11"/>
       <c r="L276" s="11"/>
       <c r="N276" s="2"/>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A277" s="7"/>
       <c r="K277" s="11"/>
       <c r="L277" s="11"/>
       <c r="N277" s="2"/>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A278" s="7"/>
       <c r="K278" s="11"/>
       <c r="L278" s="11"/>
       <c r="N278" s="2"/>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A279" s="7"/>
       <c r="K279" s="11"/>
       <c r="L279" s="11"/>
       <c r="N279" s="2"/>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A280" s="14"/>
       <c r="K280" s="11"/>
       <c r="L280" s="11"/>
       <c r="N280" s="2"/>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A281" s="14"/>
       <c r="K281" s="11"/>
       <c r="L281" s="11"/>
       <c r="N281" s="2"/>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K282" s="11"/>
       <c r="L282" s="11"/>
       <c r="N282" s="2"/>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K283" s="11"/>
       <c r="L283" s="11"/>
       <c r="N283" s="2"/>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K284" s="11"/>
       <c r="L284" s="11"/>
       <c r="N284" s="2"/>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K285" s="11"/>
       <c r="L285" s="11"/>
       <c r="N285" s="2"/>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K286" s="11"/>
       <c r="L286" s="10"/>
       <c r="N286" s="2"/>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K287" s="11"/>
       <c r="L287" s="11"/>
       <c r="N287" s="2"/>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K288" s="11"/>
       <c r="L288" s="11"/>
       <c r="N288" s="2"/>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K289" s="11"/>
       <c r="L289" s="11"/>
       <c r="N289" s="2"/>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K290" s="11"/>
       <c r="L290" s="11"/>
       <c r="N290" s="2"/>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K291" s="11"/>
       <c r="L291" s="11"/>
       <c r="N291" s="2"/>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K292" s="11"/>
       <c r="L292" s="11"/>
       <c r="N292" s="2"/>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K293" s="11"/>
       <c r="L293" s="11"/>
       <c r="N293" s="2"/>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K294" s="11"/>
       <c r="L294" s="11"/>
       <c r="N294" s="2"/>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K295" s="11"/>
       <c r="L295" s="11"/>
       <c r="N295" s="2"/>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296" s="7"/>
       <c r="K296" s="11"/>
       <c r="L296" s="11"/>
       <c r="N296" s="2"/>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A297" s="7"/>
       <c r="K297" s="11"/>
       <c r="L297" s="10"/>
       <c r="N297" s="2"/>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A298" s="7"/>
       <c r="K298" s="11"/>
       <c r="L298" s="11"/>
       <c r="N298" s="2"/>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299" s="7"/>
       <c r="K299" s="11"/>
       <c r="L299" s="11"/>
       <c r="N299" s="2"/>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A300" s="7"/>
       <c r="K300" s="11"/>
       <c r="L300" s="11"/>
       <c r="N300" s="2"/>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301" s="7"/>
       <c r="K301" s="11"/>
       <c r="L301" s="11"/>
       <c r="N301" s="2"/>
     </row>
-    <row r="302" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K302" s="11"/>
       <c r="N302" s="2"/>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K303" s="11"/>
       <c r="N303" s="2"/>
     </row>
-    <row r="304" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K304" s="11"/>
       <c r="N304" s="2"/>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K305" s="11"/>
       <c r="N305" s="2"/>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
       <c r="K306" s="11"/>
       <c r="L306" s="11"/>
       <c r="N306" s="2"/>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A307" s="7"/>
       <c r="K307" s="11"/>
       <c r="L307" s="11"/>
       <c r="N307" s="2"/>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A308" s="7"/>
       <c r="K308" s="11"/>
       <c r="L308" s="11"/>
       <c r="N308" s="2"/>
     </row>
-    <row r="309" spans="1:14" x14ac:dyDescent="0.3">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309" s="7"/>
       <c r="K309" s="11"/>
       <c r="L309" s="11"/>
       <c r="N309" s="2"/>
     </row>
-    <row r="1048565" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1048565" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1048565" s="8"/>
     </row>
   </sheetData>

</xml_diff>